<commit_message>
Added important columns to new spreadsheet, made a copy of the original
</commit_message>
<xml_diff>
--- a/Deidentified Aneurysm Genetics Study Database_20200601.xlsx
+++ b/Deidentified Aneurysm Genetics Study Database_20200601.xlsx
@@ -2242,7 +2242,7 @@
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.5"/>
@@ -2636,11 +2636,11 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.65"/>
@@ -8669,17 +8669,17 @@
   </sheetPr>
   <dimension ref="A1:S98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="29.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.65"/>
@@ -13709,7 +13709,7 @@
       <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.83"/>
@@ -14260,7 +14260,7 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.33"/>
@@ -14323,7 +14323,7 @@
       <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="27.85"/>

</xml_diff>